<commit_message>
changes in the code
</commit_message>
<xml_diff>
--- a/Latency_Data.xlsx
+++ b/Latency_Data.xlsx
@@ -411,206 +411,206 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>0.9852426213106553</v>
+        <v>0.8786531130876747</v>
       </c>
       <c r="B2">
-        <v>1686901053.278499</v>
+        <v>1690542149.590441</v>
       </c>
       <c r="C2">
-        <v>0.4302597753641374</v>
+        <v>0.7458539710474285</v>
       </c>
       <c r="D2">
-        <v>1686901053.198482</v>
+        <v>1690542149.621165</v>
       </c>
       <c r="E2">
-        <v>0.0800168514251709</v>
+        <v>0.03072357177734375</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>0.963231615807904</v>
+        <v>0.201715374841169</v>
       </c>
       <c r="B3">
-        <v>1686901058.058773</v>
+        <v>1690542154.481643</v>
       </c>
       <c r="C3">
-        <v>0.3252175125148914</v>
+        <v>0.2189853687045643</v>
       </c>
       <c r="D3">
-        <v>1686901058.136886</v>
+        <v>1690542154.541678</v>
       </c>
       <c r="E3">
-        <v>0.07811355590820312</v>
+        <v>0.06003522872924805</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>0.9584792396198099</v>
+        <v>0.5279542566709021</v>
       </c>
       <c r="B4">
-        <v>1686901063.027271</v>
+        <v>1690542159.485935</v>
       </c>
       <c r="C4">
-        <v>0.3976611044371293</v>
+        <v>0.7797755126102133</v>
       </c>
       <c r="D4">
-        <v>1686901063.184335</v>
+        <v>1690542159.561282</v>
       </c>
       <c r="E4">
-        <v>0.1570632457733154</v>
+        <v>0.07534694671630859</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>0.975487743871936</v>
+        <v>0.6956797966963151</v>
       </c>
       <c r="B5">
-        <v>1686901068.105141</v>
+        <v>1690542164.496362</v>
       </c>
       <c r="C5">
-        <v>0.3314132693947677</v>
+        <v>0.6288722801249005</v>
       </c>
       <c r="D5">
-        <v>1686901068.21578</v>
+        <v>1690542164.551006</v>
       </c>
       <c r="E5">
-        <v>0.1106390953063965</v>
+        <v>0.05464363098144531</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>0.9779889944972487</v>
+        <v>0.4628335451080051</v>
       </c>
       <c r="B6">
-        <v>1686901073.101491</v>
+        <v>1690542169.471658</v>
       </c>
       <c r="C6">
-        <v>0.3004044455336577</v>
+        <v>0.4350479427603577</v>
       </c>
       <c r="D6">
-        <v>1686901073.116719</v>
+        <v>1690542169.541372</v>
       </c>
       <c r="E6">
-        <v>0.0152277946472168</v>
+        <v>0.06971311569213867</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>0.9804902451225613</v>
+        <v>0.4348792884371029</v>
       </c>
       <c r="B7">
-        <v>1686901078.159178</v>
+        <v>1690542174.489388</v>
       </c>
       <c r="C7">
-        <v>0.3406834808446455</v>
+        <v>0.2487097363452859</v>
       </c>
       <c r="D7">
-        <v>1686901078.142563</v>
+        <v>1690542174.541356</v>
       </c>
       <c r="E7">
-        <v>0.01661562919616699</v>
+        <v>0.05196833610534668</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>0.9657328664332167</v>
+        <v>0.6489834815756035</v>
       </c>
       <c r="B8">
-        <v>1686901083.054151</v>
+        <v>1690542179.48918</v>
       </c>
       <c r="C8">
-        <v>0.3290915054435589</v>
+        <v>0.7797306323859806</v>
       </c>
       <c r="D8">
-        <v>1686901083.132649</v>
+        <v>1690542179.551663</v>
       </c>
       <c r="E8">
-        <v>0.07849812507629395</v>
+        <v>0.06248378753662109</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>0.963231615807904</v>
+        <v>0.3538754764930114</v>
       </c>
       <c r="B9">
-        <v>1686901088.053082</v>
+        <v>1690542184.469036</v>
       </c>
       <c r="C9">
-        <v>0.3070165807352661</v>
+        <v>0.3348395081812096</v>
       </c>
       <c r="D9">
-        <v>1686901088.115478</v>
+        <v>1690542184.537835</v>
       </c>
       <c r="E9">
-        <v>0.06239533424377441</v>
+        <v>0.06879878044128418</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>0.9682341170585292</v>
+        <v>0.6022871664548919</v>
       </c>
       <c r="B10">
-        <v>1686901093.061429</v>
+        <v>1690542189.487218</v>
       </c>
       <c r="C10">
-        <v>0.3108359938208484</v>
+        <v>0.3516973899359572</v>
       </c>
       <c r="D10">
-        <v>1686901093.202761</v>
+        <v>1690542188.857749</v>
       </c>
       <c r="E10">
-        <v>0.141331672668457</v>
+        <v>0.6294693946838379</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>0.9609804902451226</v>
+        <v>0.7420584498094027</v>
       </c>
       <c r="B11">
-        <v>1686901098.048123</v>
+        <v>1690542194.481706</v>
       </c>
       <c r="C11">
-        <v>0.3932900641373649</v>
+        <v>0.6957297099963836</v>
       </c>
       <c r="D11">
-        <v>1686901098.173915</v>
+        <v>1690542194.547652</v>
       </c>
       <c r="E11">
-        <v>0.1257920265197754</v>
+        <v>0.06594562530517578</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>0.9512256128064033</v>
+        <v>0.5403430749682337</v>
       </c>
       <c r="B12">
-        <v>1686901103.006166</v>
+        <v>1690542199.485257</v>
       </c>
       <c r="C12">
-        <v>0.3264338835444329</v>
+        <v>0.4861224937766774</v>
       </c>
       <c r="D12">
-        <v>1686901103.115986</v>
+        <v>1690542199.537884</v>
       </c>
       <c r="E12">
-        <v>0.1098196506500244</v>
+        <v>0.0526275634765625</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>0.975487743871936</v>
+        <v>0.633418043202033</v>
       </c>
       <c r="B13">
-        <v>1686901108.093077</v>
+        <v>1690542204.494275</v>
       </c>
       <c r="C13">
-        <v>0.3147489947420695</v>
+        <v>0.2552589284259358</v>
       </c>
       <c r="D13">
-        <v>1686901108.108153</v>
+        <v>1690542204.527619</v>
       </c>
       <c r="E13">
-        <v>0.0150763988494873</v>
+        <v>0.03334403038024902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>